<commit_message>
fix add form input handling
store day and time values into db

Resolves: #3
</commit_message>
<xml_diff>
--- a/doc/BUG-TRACKING.xlsx
+++ b/doc/BUG-TRACKING.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>STATUS</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>Allow db to store extra values in add couse form</t>
+  </si>
+  <si>
+    <t>bug</t>
+  </si>
+  <si>
+    <t>fix scrolling capability in time entry</t>
+  </si>
+  <si>
+    <t>feature request</t>
+  </si>
+  <si>
+    <t>allow CRUD operations on course data</t>
   </si>
 </sst>
 </file>
@@ -394,15 +406,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
     <col min="4" max="4" width="57.140625" customWidth="1"/>
   </cols>
@@ -447,6 +459,34 @@
       </c>
       <c r="D3" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>